<commit_message>
feat: módulo Administración Usuario
</commit_message>
<xml_diff>
--- a/Catalogos.xlsx
+++ b/Catalogos.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>catalogo</t>
   </si>
@@ -184,6 +183,66 @@
   </si>
   <si>
     <t>inputs text</t>
+  </si>
+  <si>
+    <t>fecha ingreso Magisterio</t>
+  </si>
+  <si>
+    <t>fecha ingreso Institución</t>
+  </si>
+  <si>
+    <t>Actividad Laboral</t>
+  </si>
+  <si>
+    <t>Docente</t>
+  </si>
+  <si>
+    <t>DECE</t>
+  </si>
+  <si>
+    <t>Autoridad</t>
+  </si>
+  <si>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>Preparatoria</t>
+  </si>
+  <si>
+    <t>Elemental</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Superior</t>
+  </si>
+  <si>
+    <t>Bachillerato</t>
+  </si>
+  <si>
+    <t>PCEI no Intensivo</t>
+  </si>
+  <si>
+    <t>PCEI Intensivo</t>
+  </si>
+  <si>
+    <t>Nacionalidad Indígena</t>
+  </si>
+  <si>
+    <t>sexo</t>
+  </si>
+  <si>
+    <t>si/no Jubilado</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Observación</t>
+  </si>
+  <si>
+    <t>text area</t>
   </si>
 </sst>
 </file>
@@ -221,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +333,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -304,7 +381,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
@@ -343,6 +420,18 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
@@ -625,31 +714,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:K52"/>
+  <dimension ref="A4:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
+    <col min="11" max="11" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -665,7 +755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>1</v>
       </c>
@@ -686,7 +776,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>2</v>
       </c>
@@ -709,7 +799,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>3</v>
       </c>
@@ -732,7 +822,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>4</v>
       </c>
@@ -752,7 +842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>5</v>
       </c>
@@ -771,8 +861,11 @@
       <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>6</v>
       </c>
@@ -791,8 +884,11 @@
       <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>7</v>
       </c>
@@ -812,7 +908,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
         <v>8</v>
       </c>
@@ -823,8 +919,11 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>9</v>
       </c>
@@ -834,8 +933,11 @@
       <c r="D14" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>10</v>
       </c>
@@ -845,8 +947,14 @@
       <c r="D15" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>11</v>
       </c>
@@ -855,6 +963,12 @@
       </c>
       <c r="D16" s="8">
         <v>8</v>
+      </c>
+      <c r="K16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L16" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -1036,7 +1150,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>28</v>
       </c>
@@ -1047,7 +1161,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>29</v>
       </c>
@@ -1058,7 +1172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>30</v>
       </c>
@@ -1069,7 +1183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="16">
         <v>31</v>
       </c>
@@ -1081,7 +1195,7 @@
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>32</v>
       </c>
@@ -1092,7 +1206,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>33</v>
       </c>
@@ -1102,8 +1216,11 @@
       <c r="D38" s="5">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>34</v>
       </c>
@@ -1114,7 +1231,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>35</v>
       </c>
@@ -1125,7 +1242,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>36</v>
       </c>
@@ -1136,7 +1253,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>37</v>
       </c>
@@ -1147,54 +1264,264 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="19">
         <v>38</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" s="20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46">
         <v>41</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47">
+      <c r="C46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="21">
         <v>42</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48">
         <v>43</v>
       </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D48" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>44</v>
       </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
         <v>45</v>
       </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D50" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3">
         <v>47</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>48</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>49</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54" s="21">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ft: administracion de usuarios
</commit_message>
<xml_diff>
--- a/Catalogos.xlsx
+++ b/Catalogos.xlsx
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>